<commit_message>
Starship explosion not working propperly
</commit_message>
<xml_diff>
--- a/assets/Pygame_shapes.xlsx
+++ b/assets/Pygame_shapes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/federico.tognetti/Python_Portfolio_Projects/14_Space_Invaders/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD2A5912-91BC-0C43-9C44-ACDEFE33FFB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24CE0BA6-D026-9A47-9D41-5086D61D1639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{9720652C-E0D3-6543-921A-B0F9550DEC2C}"/>
   </bookViews>
@@ -540,7 +540,7 @@
   <dimension ref="B1:AY26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AC1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="BL16" sqref="BL15:BL16"/>
+      <selection activeCell="AO3" sqref="AO3:AY12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>